<commit_message>
working on specialization list & detail
</commit_message>
<xml_diff>
--- a/assets/res/tables_data.xlsx
+++ b/assets/res/tables_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -40,9 +40,6 @@
     <t xml:space="preserve">password</t>
   </si>
   <si>
-    <t xml:space="preserve">hub_ids</t>
-  </si>
-  <si>
     <t xml:space="preserve">specialization_ids</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
     <t xml:space="preserve">Pratik Joshi</t>
   </si>
   <si>
+    <t xml:space="preserve">9909990132</t>
+  </si>
+  <si>
     <t xml:space="preserve">Male</t>
   </si>
   <si>
@@ -64,15 +64,15 @@
     <t xml:space="preserve">PJ@123</t>
   </si>
   <si>
-    <t xml:space="preserve">DC02</t>
-  </si>
-  <si>
     <t xml:space="preserve">DB02</t>
   </si>
   <si>
     <t xml:space="preserve">Gaurav Balbhadra</t>
   </si>
   <si>
+    <t xml:space="preserve">7990357110</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gota </t>
   </si>
   <si>
@@ -85,19 +85,22 @@
     <t xml:space="preserve">Mansi Joshi</t>
   </si>
   <si>
+    <t xml:space="preserve">9753555363</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gota</t>
   </si>
   <si>
     <t xml:space="preserve">Test@12</t>
   </si>
   <si>
-    <t xml:space="preserve">DC01</t>
-  </si>
-  <si>
     <t xml:space="preserve">DB03</t>
   </si>
   <si>
     <t xml:space="preserve">IT Tester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8790818948</t>
   </si>
   <si>
     <t xml:space="preserve">Female</t>
@@ -212,20 +215,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L37" activeCellId="0" sqref="L37"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -250,19 +254,16 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>9909990131</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>10</v>
@@ -279,19 +280,16 @@
       <c r="G2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="1" t="n">
+      <c r="H2" s="1" t="n">
         <v>2018</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>7990377110</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>10</v>
@@ -306,12 +304,9 @@
         <v>18</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="H3" s="1" t="n">
         <v>2020</v>
       </c>
     </row>
@@ -319,8 +314,8 @@
       <c r="A4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="1" t="n">
-        <v>9723555363</v>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
         <v>10</v>
@@ -329,18 +324,15 @@
         <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="H4" s="1" t="n">
         <v>2018</v>
       </c>
     </row>
@@ -348,17 +340,17 @@
       <c r="A5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="n">
-        <v>8780818948</v>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="2" t="n">
         <v>12345678</v>
@@ -366,10 +358,7 @@
       <c r="G5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="1" t="n">
+      <c r="H5" s="1" t="n">
         <v>2017</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add email filed in multiple student , resolve scrolling issue
</commit_message>
<xml_diff>
--- a/assets/res/tables_data.xlsx
+++ b/assets/res/tables_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">division</t>
   </si>
   <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pratik Joshi</t>
   </si>
   <si>
@@ -74,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Class A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gb@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -84,7 +90,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -105,6 +111,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -149,12 +162,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,10 +192,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="topLeft" activeCell="K37" activeCellId="0" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -190,7 +207,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="16.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="12" style="1" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -224,28 +243,31 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="n">
         <v>2018</v>
@@ -254,10 +276,16 @@
         <v>1</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" display="gb@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
student request model updated
</commit_message>
<xml_diff>
--- a/assets/res/tables_data.xlsx
+++ b/assets/res/tables_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -37,6 +37,9 @@
     <t xml:space="preserve">address</t>
   </si>
   <si>
+    <t xml:space="preserve">pin_code</t>
+  </si>
+  <si>
     <t xml:space="preserve">hub_ids</t>
   </si>
   <si>
@@ -46,13 +49,43 @@
     <t xml:space="preserve">joining_year</t>
   </si>
   <si>
+    <t xml:space="preserve">email</t>
+  </si>
+  <si>
     <t xml:space="preserve">semester</t>
   </si>
   <si>
     <t xml:space="preserve">division</t>
   </si>
   <si>
-    <t xml:space="preserve">email</t>
+    <t xml:space="preserve">sr_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birthdate(dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aadhar_card_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">caste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsc_school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsc_school_city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hsc_percentage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mother_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mother_number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">father_number</t>
   </si>
   <si>
     <t xml:space="preserve">Pratik Joshi</t>
@@ -70,16 +103,46 @@
     <t xml:space="preserve">Adani shantigram</t>
   </si>
   <si>
+    <t xml:space="preserve">382481</t>
+  </si>
+  <si>
     <t xml:space="preserve">DC014</t>
   </si>
   <si>
     <t xml:space="preserve">DB011</t>
   </si>
   <si>
+    <t xml:space="preserve">gb@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">Class A</t>
   </si>
   <si>
-    <t xml:space="preserve">gb@gmail.com</t>
+    <t xml:space="preserve">18/09/1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">987654321032</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brahmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Navyug School</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porbandar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Madhuben</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543210</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9876543212</t>
   </si>
 </sst>
 </file>
@@ -192,10 +255,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -204,12 +267,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="1" width="16.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.86"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="11.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="19.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="12" style="1" width="11.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="1" width="16.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="11" style="1" width="11.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="19.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="19.86"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="16" style="1" width="11.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="14.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="19.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="23" style="1" width="11.64"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,45 +317,111 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="1" t="n">
         <v>2018</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="J2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
+      <c r="L2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" display="gb@gmail.com"/>
+    <hyperlink ref="J2" r:id="rId1" display="gb@gmail.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Attendance and Placement module changes
</commit_message>
<xml_diff>
--- a/assets/res/tables_data.xlsx
+++ b/assets/res/tables_data.xlsx
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Pratik Joshi</t>
   </si>
   <si>
-    <t xml:space="preserve">9909990132</t>
+    <t xml:space="preserve">8735943527</t>
   </si>
   <si>
     <t xml:space="preserve">Male</t>
@@ -257,8 +257,8 @@
   </sheetPr>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W1" activeCellId="0" sqref="W1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>